<commit_message>
Inserting admin after db creation imagePath can be longer (50 was not enough)
</commit_message>
<xml_diff>
--- a/Backend/CarGalleryAPI/CarGalleryAPI/CarGalleryDBData.xlsx
+++ b/Backend/CarGalleryAPI/CarGalleryAPI/CarGalleryDBData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frien\Desktop\CarGallery\Backend\CarGalleryAPI\CarGalleryAPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70840A8F-6ED1-4DEC-9B29-229B29D6881E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68787332-C8E6-4808-87DA-9F5BC91DF023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fuels" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -124,9 +123,6 @@
     <t>Citroen</t>
   </si>
   <si>
-    <t>DOdge</t>
-  </si>
-  <si>
     <t>Ferrari</t>
   </si>
   <si>
@@ -209,6 +205,9 @@
   </si>
   <si>
     <t>User</t>
+  </si>
+  <si>
+    <t>Dodge</t>
   </si>
 </sst>
 </file>
@@ -755,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF94CBC2-DF2F-4DDF-BC9F-6FB9AA77E26E}">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,7 +857,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -866,7 +865,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -874,7 +873,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -882,7 +881,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -890,7 +889,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -898,7 +897,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -906,7 +905,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -914,7 +913,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -930,7 +929,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -938,7 +937,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -946,7 +945,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -954,7 +953,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -962,7 +961,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -970,7 +969,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -978,7 +977,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -986,7 +985,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -994,7 +993,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -1002,7 +1001,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1010,7 +1009,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1018,7 +1017,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1026,7 +1025,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1034,7 +1033,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -1042,7 +1041,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1050,7 +1049,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1058,7 +1057,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1066,7 +1065,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1078,7 +1077,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5E430C4-E384-41BB-97AB-771A7A3C765A}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -1101,7 +1100,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1109,7 +1108,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1117,7 +1116,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>